<commit_message>
ADD : huuu,hogehoge DEL : hoge
</commit_message>
<xml_diff>
--- a/binaries/list.xlsx
+++ b/binaries/list.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>name</t>
     <phoneticPr fontId="2"/>
@@ -57,11 +57,15 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>F</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>O</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>hoge4</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>T</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -424,16 +428,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="20" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -478,7 +480,18 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="B5" s="1">
+        <v>100</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>